<commit_message>
Clean up datasheet columns
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@22319 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/Processors.xlsx
+++ b/Digikey/Processors.xlsx
@@ -2056,7 +2056,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2066,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
@@ -2603,7 +2603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="AE2" sqref="AE2:AE6"/>
     </sheetView>
   </sheetViews>
@@ -3178,7 +3178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
@@ -3999,7 +3999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>

</xml_diff>